<commit_message>
Planilha de tarefas e codigo de leitura de vtk
</commit_message>
<xml_diff>
--- a/TCC tasks.xlsx
+++ b/TCC tasks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Desktop\TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61DA1DD-8B3F-4D61-AE96-F1FD60C79BFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D193A7-EFB2-4FE1-992C-5AAF25FA3FE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Validação 3D Ansys</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>Verificar se dá pra resolver o "Thermal stress"</t>
+  </si>
+  <si>
+    <t>O algoritmo</t>
+  </si>
+  <si>
+    <t>Solução analítica 3D (Ansys)</t>
+  </si>
+  <si>
+    <t>Conclusões</t>
   </si>
 </sst>
 </file>
@@ -381,7 +390,7 @@
   <dimension ref="B1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,15 +439,24 @@
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>